<commit_message>
merge remote main into local
</commit_message>
<xml_diff>
--- a/parameters/gen_new/factors.xlsx
+++ b/parameters/gen_new/factors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="11540"/>
+    <workbookView windowWidth="27660" windowHeight="11540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eps_factors" sheetId="2" r:id="rId1"/>
@@ -1189,8 +1189,8 @@
   <sheetPr/>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1588,10 +1588,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>0.338981607240582</v>
+        <v>0.119521198487387</v>
       </c>
       <c r="B24">
-        <v>1.44738656748225</v>
+        <v>0.120600956941548</v>
       </c>
       <c r="C24">
         <v>0.177073948661523</v>
@@ -1648,8 +1648,8 @@
   <sheetPr/>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2047,10 +2047,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>0.043211</v>
+        <v>0.404433</v>
       </c>
       <c r="B24">
-        <v>-0.0609312</v>
+        <v>0.2579358</v>
       </c>
       <c r="C24">
         <v>0.2434472</v>

</xml_diff>